<commit_message>
Figures and Tables generated from code
</commit_message>
<xml_diff>
--- a/ms/Accessory/Sup_TableXX_flowering_parts_categories_descriptions_methods.xlsx
+++ b/ms/Accessory/Sup_TableXX_flowering_parts_categories_descriptions_methods.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mq20111250\Documents\RA schedules - Kuringgai research\Reproductive_Allocation_Kuringgai\ms\Accessory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mq20111250\Documents\Reproductive_Allocation_Kuringgai\ms\Accessory\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="262">
   <si>
     <t>Banksia ericifolia</t>
   </si>
@@ -792,6 +792,24 @@
   </si>
   <si>
     <t>ovules per unit</t>
+  </si>
+  <si>
+    <t>pollen-attraction and packaging and dispersal</t>
+  </si>
+  <si>
+    <t>discarded pollen-attraction</t>
+  </si>
+  <si>
+    <t>discarded packaging and dispersal</t>
+  </si>
+  <si>
+    <t>discarded pollen-attraction and discarded packaging and dispersal</t>
+  </si>
+  <si>
+    <t>reproductive investment pool(s)</t>
+  </si>
+  <si>
+    <t>successful pollen-attraction (and discarded pollen-attraction)</t>
   </si>
 </sst>
 </file>
@@ -1231,10 +1249,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E286"/>
+  <dimension ref="A1:F286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
-      <selection activeCell="L152" sqref="L152"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,14 +1262,15 @@
     <col min="3" max="3" width="22.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -1267,8 +1286,11 @@
       <c r="E2" s="14" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1284,8 +1306,11 @@
       <c r="E3" s="16">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1301,8 +1326,11 @@
       <c r="E4" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1318,8 +1346,11 @@
       <c r="E5" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1335,8 +1366,11 @@
       <c r="E6" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1352,8 +1386,11 @@
       <c r="E7" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -1369,8 +1406,11 @@
       <c r="E8" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -1386,8 +1426,11 @@
       <c r="E9" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1403,8 +1446,11 @@
       <c r="E10" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1420,8 +1466,11 @@
       <c r="E11" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1437,8 +1486,11 @@
       <c r="E12" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1454,8 +1506,11 @@
       <c r="E13" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1471,8 +1526,11 @@
       <c r="E14" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -1489,7 +1547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
@@ -1506,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -1523,7 +1581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -1539,8 +1597,11 @@
       <c r="E18" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
@@ -1556,8 +1617,11 @@
       <c r="E19" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
@@ -1573,8 +1637,11 @@
       <c r="E20" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -1590,8 +1657,11 @@
       <c r="E21" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
@@ -1607,8 +1677,11 @@
       <c r="E22" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
@@ -1624,8 +1697,11 @@
       <c r="E23" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
@@ -1641,8 +1717,11 @@
       <c r="E24" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
@@ -1658,8 +1737,11 @@
       <c r="E25" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
@@ -1675,8 +1757,11 @@
       <c r="E26" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
@@ -1692,8 +1777,11 @@
       <c r="E27" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
@@ -1709,8 +1797,11 @@
       <c r="E28" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
@@ -1726,8 +1817,11 @@
       <c r="E29" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
@@ -1743,8 +1837,11 @@
       <c r="E30" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>29</v>
       </c>
@@ -1760,8 +1857,11 @@
       <c r="E31" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>30</v>
       </c>
@@ -1777,8 +1877,11 @@
       <c r="E32" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>31</v>
       </c>
@@ -1794,13 +1897,16 @@
       <c r="E33" s="19">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>32</v>
       </c>
@@ -1817,7 +1923,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>1</v>
       </c>
@@ -1834,7 +1940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>2</v>
       </c>
@@ -1851,7 +1957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>3</v>
       </c>
@@ -1868,7 +1974,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>4</v>
       </c>
@@ -1885,7 +1991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>6</v>
       </c>
@@ -1902,7 +2008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>77</v>
       </c>
@@ -1919,7 +2025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>78</v>
       </c>
@@ -1936,7 +2042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>9</v>
       </c>
@@ -1953,7 +2059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>79</v>
       </c>
@@ -1970,7 +2076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>80</v>
       </c>
@@ -1987,7 +2093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>10</v>
       </c>
@@ -2004,7 +2110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>11</v>
       </c>

</xml_diff>